<commit_message>
Create specific dictionary for hospit export in TZ
</commit_message>
<xml_diff>
--- a/inst/extdata/hospit_dict.xlsx
+++ b/inst/extdata/hospit_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="116">
   <si>
     <t>old</t>
   </si>
@@ -363,6 +363,15 @@
   </si>
   <si>
     <t>start</t>
+  </si>
+  <si>
+    <t>meta-instanceID</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>instanceID</t>
   </si>
 </sst>
 </file>
@@ -415,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -442,6 +451,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1310,6 +1322,20 @@
         <v>111</v>
       </c>
     </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Prepare for change in dictionaries
</commit_message>
<xml_diff>
--- a/inst/extdata/hospit_dict.xlsx
+++ b/inst/extdata/hospit_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="129">
   <si>
     <t>old</t>
   </si>
@@ -378,32 +378,72 @@
   </si>
   <si>
     <t>form_version</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>is_tanzania</t>
+  </si>
+  <si>
+    <t>a1-rfid</t>
+  </si>
+  <si>
+    <t>is_india</t>
+  </si>
+  <si>
+    <t>is_kenya</t>
+  </si>
+  <si>
+    <t>is_senegal</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -414,6 +454,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,21 +488,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -456,18 +511,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -743,49 +835,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.58203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.75" style="5" customWidth="1"/>
+    <col min="9" max="9" width="9.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -795,571 +920,1259 @@
       <c r="C3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B11" s="7">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B10">
+      <c r="B12" s="7">
         <v>0</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B14" s="7">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B15" s="7">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B14">
+      <c r="B16" s="7">
         <v>0</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C16" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" s="5">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B15">
+      <c r="B17" s="7">
         <v>0</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B17">
+      <c r="B19" s="7">
         <v>0</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B20" s="7">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="E20" s="5">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="E21" s="5">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B22" s="7">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="E22" s="5">
+        <v>1</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B23" s="7">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="E23" s="5">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B24" s="7">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="E24" s="5">
+        <v>1</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B25" s="7">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="E25" s="5">
+        <v>1</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
+      <c r="H25" s="5">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="E26" s="5">
+        <v>1</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B27" s="7">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="E27" s="5">
+        <v>1</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="E28" s="5">
+        <v>1</v>
+      </c>
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="E29" s="5">
+        <v>1</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B30" s="7">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="E30" s="5">
+        <v>1</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="E31" s="5">
+        <v>1</v>
+      </c>
+      <c r="F31" s="5">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B32" s="7">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="E32" s="5">
+        <v>1</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
+      <c r="H32" s="5">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="E33" s="5">
+        <v>1</v>
+      </c>
+      <c r="F33" s="5">
+        <v>1</v>
+      </c>
+      <c r="G33" s="5">
+        <v>1</v>
+      </c>
+      <c r="H33" s="5">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B34" s="7">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="E34" s="5">
+        <v>1</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5">
+        <v>1</v>
+      </c>
+      <c r="H34" s="5">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="B35" s="7">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="E35" s="5">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="5">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="B36" s="7">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="E36" s="5">
+        <v>1</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5">
+        <v>1</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="E37" s="5">
+        <v>1</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5">
+        <v>1</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B38" s="7">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D38" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="E38" s="5">
+        <v>1</v>
+      </c>
+      <c r="F38" s="5">
+        <v>1</v>
+      </c>
+      <c r="G38" s="5">
+        <v>1</v>
+      </c>
+      <c r="H38" s="5">
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="E39" s="5">
+        <v>1</v>
+      </c>
+      <c r="F39" s="5">
+        <v>1</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="B40" s="7">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="E40" s="5">
+        <v>1</v>
+      </c>
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
+      <c r="H40" s="5">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="B41" s="7">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D41" s="6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="E41" s="5">
+        <v>1</v>
+      </c>
+      <c r="F41" s="5">
+        <v>1</v>
+      </c>
+      <c r="G41" s="5">
+        <v>1</v>
+      </c>
+      <c r="H41" s="5">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="B42" s="7">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D42" s="6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="E42" s="5">
+        <v>1</v>
+      </c>
+      <c r="F42" s="5">
+        <v>1</v>
+      </c>
+      <c r="G42" s="5">
+        <v>1</v>
+      </c>
+      <c r="H42" s="5">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="B43" s="7">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="E43" s="5">
+        <v>1</v>
+      </c>
+      <c r="F43" s="5">
+        <v>1</v>
+      </c>
+      <c r="G43" s="5">
+        <v>1</v>
+      </c>
+      <c r="H43" s="5">
+        <v>1</v>
+      </c>
+      <c r="I43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B42" s="9">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B44" s="6">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D44" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="E44" s="5">
+        <v>1</v>
+      </c>
+      <c r="F44" s="5">
+        <v>1</v>
+      </c>
+      <c r="G44" s="5">
+        <v>1</v>
+      </c>
+      <c r="H44" s="5">
+        <v>1</v>
+      </c>
+      <c r="I44" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B43" s="9">
-        <v>1</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="B45" s="6">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D45" s="9" t="s">
         <v>116</v>
       </c>
+      <c r="E45" s="5">
+        <v>1</v>
+      </c>
+      <c r="F45" s="5">
+        <v>1</v>
+      </c>
+      <c r="G45" s="5">
+        <v>1</v>
+      </c>
+      <c r="H45" s="5">
+        <v>1</v>
+      </c>
+      <c r="I45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46"/>
+      <c r="C46"/>
+      <c r="D46"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:H45">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B45">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update hospit_dict for rhf_id export in KE/SE
</commit_message>
<xml_diff>
--- a/inst/extdata/hospit_dict.xlsx
+++ b/inst/extdata/hospit_dict.xlsx
@@ -864,7 +864,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1130,10 +1130,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="5">
         <v>0</v>
@@ -1159,10 +1159,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
Update the hard lock for Kenya and Senegal
</commit_message>
<xml_diff>
--- a/inst/extdata/hospit_dict.xlsx
+++ b/inst/extdata/hospit_dict.xlsx
@@ -864,7 +864,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1057,7 +1057,7 @@
         <v>124</v>
       </c>
       <c r="B7" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>125</v>
@@ -1086,7 +1086,7 @@
         <v>60</v>
       </c>
       <c r="B8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Update hospit dict for Senegal
</commit_message>
<xml_diff>
--- a/inst/extdata/hospit_dict.xlsx
+++ b/inst/extdata/hospit_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="133">
   <si>
     <t>old</t>
   </si>
@@ -405,6 +405,24 @@
   </si>
   <si>
     <t>n2t-n3_1</t>
+  </si>
+  <si>
+    <t>n4_1_extended</t>
+  </si>
+  <si>
+    <t>n4-n4_1_extended</t>
+  </si>
+  <si>
+    <t>dx_admission_ext</t>
+  </si>
+  <si>
+    <t>n4-n4_8_extended</t>
+  </si>
+  <si>
+    <t>dx_discharge_ext</t>
+  </si>
+  <si>
+    <t>n4_8_extended</t>
   </si>
 </sst>
 </file>
@@ -524,7 +542,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -861,24 +939,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.375" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.25" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="9.75" style="5" customWidth="1"/>
     <col min="9" max="9" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -907,7 +985,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -936,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>111</v>
       </c>
@@ -965,7 +1043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>117</v>
       </c>
@@ -994,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1023,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1052,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
@@ -1081,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>60</v>
       </c>
@@ -1110,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -1139,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>119</v>
       </c>
@@ -1168,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -1197,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -1226,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>36</v>
       </c>
@@ -1255,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1284,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
@@ -1313,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -1342,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>40</v>
       </c>
@@ -1371,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>41</v>
       </c>
@@ -1400,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -1429,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>43</v>
       </c>
@@ -1458,7 +1536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1487,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -1516,7 +1594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
@@ -1545,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1574,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -1603,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>126</v>
       </c>
@@ -1632,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
@@ -1661,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>50</v>
       </c>
@@ -1690,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>51</v>
       </c>
@@ -1719,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>52</v>
       </c>
@@ -1748,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>53</v>
       </c>
@@ -1777,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>54</v>
       </c>
@@ -1806,439 +1884,512 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0</v>
+      </c>
+      <c r="H33" s="5">
+        <v>1</v>
+      </c>
+      <c r="I33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="7">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B34" s="7">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E33" s="5">
-        <v>1</v>
-      </c>
-      <c r="F33" s="5">
-        <v>1</v>
-      </c>
-      <c r="G33" s="5">
-        <v>1</v>
-      </c>
-      <c r="H33" s="5">
-        <v>1</v>
-      </c>
-      <c r="I33" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="E34" s="5">
+        <v>1</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5">
+        <v>1</v>
+      </c>
+      <c r="H34" s="5">
+        <v>1</v>
+      </c>
+      <c r="I34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="7">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B35" s="7">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="5">
-        <v>1</v>
-      </c>
-      <c r="F34" s="5">
-        <v>1</v>
-      </c>
-      <c r="G34" s="5">
-        <v>1</v>
-      </c>
-      <c r="H34" s="5">
-        <v>1</v>
-      </c>
-      <c r="I34" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="E35" s="5">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="5">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5">
+        <v>1</v>
+      </c>
+      <c r="I35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="7">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B36" s="7">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="5">
-        <v>1</v>
-      </c>
-      <c r="F35" s="5">
-        <v>1</v>
-      </c>
-      <c r="G35" s="5">
-        <v>1</v>
-      </c>
-      <c r="H35" s="5">
-        <v>1</v>
-      </c>
-      <c r="I35" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="E36" s="5">
+        <v>1</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5">
+        <v>1</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1</v>
+      </c>
+      <c r="I36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="7">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="5">
-        <v>1</v>
-      </c>
-      <c r="F36" s="5">
-        <v>1</v>
-      </c>
-      <c r="G36" s="5">
-        <v>1</v>
-      </c>
-      <c r="H36" s="5">
-        <v>1</v>
-      </c>
-      <c r="I36" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="E37" s="5">
+        <v>1</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5">
+        <v>1</v>
+      </c>
+      <c r="I37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="7">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="B38" s="7">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="5">
-        <v>1</v>
-      </c>
-      <c r="F37" s="5">
-        <v>1</v>
-      </c>
-      <c r="G37" s="5">
-        <v>1</v>
-      </c>
-      <c r="H37" s="5">
-        <v>1</v>
-      </c>
-      <c r="I37" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="E38" s="5">
+        <v>1</v>
+      </c>
+      <c r="F38" s="5">
+        <v>1</v>
+      </c>
+      <c r="G38" s="5">
+        <v>1</v>
+      </c>
+      <c r="H38" s="5">
+        <v>1</v>
+      </c>
+      <c r="I38" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="7">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="5">
-        <v>1</v>
-      </c>
-      <c r="F38" s="5">
-        <v>1</v>
-      </c>
-      <c r="G38" s="5">
-        <v>1</v>
-      </c>
-      <c r="H38" s="5">
-        <v>1</v>
-      </c>
-      <c r="I38" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+      <c r="E39" s="5">
+        <v>1</v>
+      </c>
+      <c r="F39" s="5">
+        <v>1</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5">
+        <v>1</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="7">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B40" s="7">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E39" s="5">
-        <v>1</v>
-      </c>
-      <c r="F39" s="5">
-        <v>1</v>
-      </c>
-      <c r="G39" s="5">
-        <v>1</v>
-      </c>
-      <c r="H39" s="5">
-        <v>1</v>
-      </c>
-      <c r="I39" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="E40" s="5">
+        <v>1</v>
+      </c>
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
+      <c r="H40" s="5">
+        <v>1</v>
+      </c>
+      <c r="I40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="7">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="B41" s="7">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E40" s="5">
-        <v>1</v>
-      </c>
-      <c r="F40" s="5">
-        <v>1</v>
-      </c>
-      <c r="G40" s="5">
-        <v>1</v>
-      </c>
-      <c r="H40" s="5">
-        <v>1</v>
-      </c>
-      <c r="I40" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="E41" s="5">
+        <v>1</v>
+      </c>
+      <c r="F41" s="5">
+        <v>1</v>
+      </c>
+      <c r="G41" s="5">
+        <v>1</v>
+      </c>
+      <c r="H41" s="5">
+        <v>1</v>
+      </c>
+      <c r="I41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="7">
-        <v>1</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="B42" s="7">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E41" s="5">
-        <v>1</v>
-      </c>
-      <c r="F41" s="5">
-        <v>1</v>
-      </c>
-      <c r="G41" s="5">
-        <v>1</v>
-      </c>
-      <c r="H41" s="5">
-        <v>1</v>
-      </c>
-      <c r="I41" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="E42" s="5">
+        <v>1</v>
+      </c>
+      <c r="F42" s="5">
+        <v>1</v>
+      </c>
+      <c r="G42" s="5">
+        <v>1</v>
+      </c>
+      <c r="H42" s="5">
+        <v>1</v>
+      </c>
+      <c r="I42" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="7">
-        <v>1</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="B43" s="7">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="5">
-        <v>1</v>
-      </c>
-      <c r="F42" s="5">
-        <v>1</v>
-      </c>
-      <c r="G42" s="5">
-        <v>1</v>
-      </c>
-      <c r="H42" s="5">
-        <v>1</v>
-      </c>
-      <c r="I42" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="E43" s="5">
+        <v>1</v>
+      </c>
+      <c r="F43" s="5">
+        <v>1</v>
+      </c>
+      <c r="G43" s="5">
+        <v>1</v>
+      </c>
+      <c r="H43" s="5">
+        <v>1</v>
+      </c>
+      <c r="I43" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" s="7">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+      <c r="H44" s="5">
+        <v>1</v>
+      </c>
+      <c r="I44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="7">
-        <v>1</v>
-      </c>
-      <c r="C43" s="4" t="s">
+      <c r="B45" s="7">
+        <v>1</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E43" s="5">
-        <v>1</v>
-      </c>
-      <c r="F43" s="5">
-        <v>1</v>
-      </c>
-      <c r="G43" s="5">
-        <v>1</v>
-      </c>
-      <c r="H43" s="5">
-        <v>1</v>
-      </c>
-      <c r="I43" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="E45" s="5">
+        <v>1</v>
+      </c>
+      <c r="F45" s="5">
+        <v>1</v>
+      </c>
+      <c r="G45" s="5">
+        <v>1</v>
+      </c>
+      <c r="H45" s="5">
+        <v>1</v>
+      </c>
+      <c r="I45" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="7">
-        <v>1</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="B46" s="7">
+        <v>1</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E44" s="5">
-        <v>1</v>
-      </c>
-      <c r="F44" s="5">
-        <v>1</v>
-      </c>
-      <c r="G44" s="5">
-        <v>1</v>
-      </c>
-      <c r="H44" s="5">
-        <v>1</v>
-      </c>
-      <c r="I44" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="E46" s="5">
+        <v>1</v>
+      </c>
+      <c r="F46" s="5">
+        <v>1</v>
+      </c>
+      <c r="G46" s="5">
+        <v>1</v>
+      </c>
+      <c r="H46" s="5">
+        <v>1</v>
+      </c>
+      <c r="I46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="6">
-        <v>1</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B47" s="6">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D47" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E45" s="5">
-        <v>1</v>
-      </c>
-      <c r="F45" s="5">
-        <v>1</v>
-      </c>
-      <c r="G45" s="5">
-        <v>1</v>
-      </c>
-      <c r="H45" s="5">
-        <v>1</v>
-      </c>
-      <c r="I45" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="E47" s="5">
+        <v>1</v>
+      </c>
+      <c r="F47" s="5">
+        <v>1</v>
+      </c>
+      <c r="G47" s="5">
+        <v>1</v>
+      </c>
+      <c r="H47" s="5">
+        <v>1</v>
+      </c>
+      <c r="I47" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B46" s="6">
-        <v>1</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B48" s="6">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D48" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E46" s="5">
-        <v>1</v>
-      </c>
-      <c r="F46" s="5">
-        <v>1</v>
-      </c>
-      <c r="G46" s="5">
-        <v>1</v>
-      </c>
-      <c r="H46" s="5">
-        <v>1</v>
-      </c>
-      <c r="I46" s="5">
+      <c r="E48" s="5">
+        <v>1</v>
+      </c>
+      <c r="F48" s="5">
+        <v>1</v>
+      </c>
+      <c r="G48" s="5">
+        <v>1</v>
+      </c>
+      <c r="H48" s="5">
+        <v>1</v>
+      </c>
+      <c r="I48" s="5">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:I6 E8:I46">
+  <conditionalFormatting sqref="E2:I6 E8:I32 E34:I43 E45:I48">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B6 B8:B43 B45:B48">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:F7 I7">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33:I33">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B6 B8:B46">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:F7 I7">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
+  <conditionalFormatting sqref="E44:I44">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="B44">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>